<commit_message>
Remove a 2030-2050 emissions constraint from Scen_SYS_CarbonBudget_Sector.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E33AB2F-1CD5-4356-AACB-93413A67D094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE601C6E-5A64-4281-8252-2A27A752F660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="159">
   <si>
     <t>LimType</t>
   </si>
@@ -549,12 +549,6 @@
     <t>UC_SCB_IND_2026-2030_Multi</t>
   </si>
   <si>
-    <t>UC_NetZero_CO2_2050_Multi</t>
-  </si>
-  <si>
-    <t>Net Zero CO2 by 2050 - Multi</t>
-  </si>
-  <si>
     <t>TRA Carbon Budget-2021-2025- Multi</t>
   </si>
   <si>
@@ -615,9 +609,6 @@
     <t>UC_SCB_IND_2026-2030_Single</t>
   </si>
   <si>
-    <t>UC_NetZero_CO2_2050_Single</t>
-  </si>
-  <si>
     <t>TRA Carbon Budget-2021-2025- Single</t>
   </si>
   <si>
@@ -646,21 +637,6 @@
   </si>
   <si>
     <t>IND Carbon Budget-2026-2030- Single</t>
-  </si>
-  <si>
-    <t>Net Zero CO2 by 2050 - Single</t>
-  </si>
-  <si>
-    <t>UC_COMNET</t>
-  </si>
-  <si>
-    <t>UC_FLO</t>
-  </si>
-  <si>
-    <t>UC_RHSRTS</t>
-  </si>
-  <si>
-    <t>UC_RHSTS</t>
   </si>
 </sst>
 </file>
@@ -918,7 +894,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,8 +974,6 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5531,10 +5505,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5549,7 +5523,7 @@
     <col min="8" max="8" width="12.265625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.59765625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.1328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.46484375" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.1328125" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.1328125" style="8"/>
   </cols>
@@ -5630,7 +5604,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>108</v>
@@ -5650,12 +5624,12 @@
       <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="19">
         <f>config!C7*1000</f>
         <v>46384.803111111105</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -5674,11 +5648,11 @@
       <c r="J8" s="8">
         <v>-1</v>
       </c>
-      <c r="K8" s="39"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>108</v>
@@ -5698,12 +5672,12 @@
       <c r="I9" s="8">
         <v>1</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="19">
         <f>config!D7*1000</f>
         <v>33159.511111111104</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -5722,11 +5696,11 @@
       <c r="J10" s="8">
         <v>-1</v>
       </c>
-      <c r="K10" s="39"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>119</v>
@@ -5746,17 +5720,17 @@
       <c r="I11" s="8">
         <v>1</v>
       </c>
-      <c r="K11" s="39">
+      <c r="K11" s="19">
         <f>config!C8*0.8*1000</f>
         <v>30662.951025777787</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>119</v>
@@ -5776,17 +5750,17 @@
       <c r="I12" s="8">
         <v>1</v>
       </c>
-      <c r="K12" s="39">
+      <c r="K12" s="19">
         <f>config!D8*0.8*1000</f>
         <v>19270.667377777783</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>120</v>
@@ -5806,17 +5780,17 @@
       <c r="I13" s="8">
         <v>1</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="19">
         <f>config!C8*0.2*1000</f>
         <v>7665.7377564444469</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>120</v>
@@ -5836,17 +5810,17 @@
       <c r="I14" s="8">
         <v>1</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="19">
         <f>config!D8*0.2*1000</f>
         <v>4817.6668444444458</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>87</v>
@@ -5866,17 +5840,17 @@
       <c r="I15" s="8">
         <v>1</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="19">
         <f>config!C6*1000</f>
         <v>41594.970666666653</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>87</v>
@@ -5896,17 +5870,17 @@
       <c r="I16" s="8">
         <v>1</v>
       </c>
-      <c r="K16" s="39">
+      <c r="K16" s="19">
         <f>config!D6*1000</f>
         <v>18047.466666666664</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B17" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>121</v>
@@ -5926,17 +5900,17 @@
       <c r="I17" s="8">
         <v>1</v>
       </c>
-      <c r="K17" s="39">
+      <c r="K17" s="19">
         <f>config!C9*1000</f>
         <v>43881.727327334855</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B18" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>121</v>
@@ -5956,154 +5930,12 @@
       <c r="I18" s="8">
         <v>1</v>
       </c>
-      <c r="K18" s="39">
+      <c r="K18" s="19">
         <f>config!D9*1000</f>
         <v>29032.066422098611</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="G23" s="8" t="str">
-        <f>IF(RIGHT(A21,1)&lt;&gt;" ","~UC_T","")</f>
-        <v>~UC_T</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B24" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" s="38"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B26" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="8">
-        <v>2030</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="8">
-        <v>1</v>
-      </c>
-      <c r="J26" s="8">
-        <v>19600</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C27" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="8">
-        <v>2030</v>
-      </c>
-      <c r="I27" s="8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C28" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="8">
-        <v>2050</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1</v>
-      </c>
-      <c r="J28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C29" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="8">
-        <v>2050</v>
-      </c>
-      <c r="I29" s="8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="F30" s="8">
-        <v>0</v>
-      </c>
-      <c r="J30" s="8">
-        <v>5</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -6115,10 +5947,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6234,12 +6066,12 @@
       <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="19">
         <f>config!C7*1000</f>
         <v>46384.803111111105</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -6258,7 +6090,7 @@
       <c r="J8" s="8">
         <v>-1</v>
       </c>
-      <c r="K8" s="39"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
@@ -6282,12 +6114,12 @@
       <c r="I9" s="8">
         <v>1</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="19">
         <f>config!D7*1000</f>
         <v>33159.511111111104</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -6306,7 +6138,7 @@
       <c r="J10" s="8">
         <v>-1</v>
       </c>
-      <c r="K10" s="39"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
@@ -6330,12 +6162,12 @@
       <c r="I11" s="8">
         <v>1</v>
       </c>
-      <c r="K11" s="39">
+      <c r="K11" s="19">
         <f>config!C8*0.8*1000</f>
         <v>30662.951025777787</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
@@ -6360,12 +6192,12 @@
       <c r="I12" s="8">
         <v>1</v>
       </c>
-      <c r="K12" s="39">
+      <c r="K12" s="19">
         <f>config!D8*0.8*1000</f>
         <v>19270.667377777783</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
@@ -6390,12 +6222,12 @@
       <c r="I13" s="8">
         <v>1</v>
       </c>
-      <c r="K13" s="39">
+      <c r="K13" s="19">
         <f>config!C8*0.2*1000</f>
         <v>7665.7377564444469</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
@@ -6420,12 +6252,12 @@
       <c r="I14" s="8">
         <v>1</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="19">
         <f>config!D8*0.2*1000</f>
         <v>4817.6668444444458</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
@@ -6450,12 +6282,12 @@
       <c r="I15" s="8">
         <v>1</v>
       </c>
-      <c r="K15" s="39">
+      <c r="K15" s="19">
         <f>config!C6*1000</f>
         <v>41594.970666666653</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
@@ -6480,12 +6312,12 @@
       <c r="I16" s="8">
         <v>1</v>
       </c>
-      <c r="K16" s="39">
+      <c r="K16" s="19">
         <f>config!D6*1000</f>
         <v>18047.466666666664</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
@@ -6510,12 +6342,12 @@
       <c r="I17" s="8">
         <v>1</v>
       </c>
-      <c r="K17" s="39">
+      <c r="K17" s="19">
         <f>config!C9*1000</f>
         <v>43881.727327334855</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
@@ -6540,154 +6372,12 @@
       <c r="I18" s="8">
         <v>1</v>
       </c>
-      <c r="K18" s="39">
+      <c r="K18" s="19">
         <f>config!D9*1000</f>
         <v>29032.066422098611</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="G23" s="8" t="str">
-        <f>IF(RIGHT(B21,1)&lt;&gt;" ","~UC_T","")</f>
-        <v>~UC_T</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B24" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B26" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="8">
-        <v>2030</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="8">
-        <v>1</v>
-      </c>
-      <c r="J26" s="8">
-        <v>19600</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C27" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="8">
-        <v>2030</v>
-      </c>
-      <c r="I27" s="8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C28" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="8">
-        <v>2050</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1</v>
-      </c>
-      <c r="J28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="C29" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="8">
-        <v>2050</v>
-      </c>
-      <c r="I29" s="8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="F30" s="8">
-        <v>0</v>
-      </c>
-      <c r="J30" s="8">
-        <v>5</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct CB budget periods
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\2022-gas-study\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF18B8F9-36B2-4868-B09F-38EEA1339FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CD8C5D-E9E9-4689-A135-50C1A802A18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="158">
   <si>
     <t>LimType</t>
   </si>
@@ -484,9 +484,6 @@
   </si>
   <si>
     <t>UC_SCB_TRA_2026-2030_Multi</t>
-  </si>
-  <si>
-    <t>2021-2026</t>
   </si>
   <si>
     <t>Electricity</t>
@@ -2239,7 +2236,7 @@
         <v>91</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
@@ -5263,7 +5260,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -5278,7 +5275,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -5291,7 +5288,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>40</v>
@@ -5302,7 +5299,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7">
         <v>54</v>
@@ -5313,7 +5310,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8">
         <v>29</v>
@@ -5324,7 +5321,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -5335,7 +5332,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10">
         <v>30</v>
@@ -5346,7 +5343,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11">
         <v>106</v>
@@ -5357,7 +5354,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -5380,7 +5377,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5473,7 +5470,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>106</v>
@@ -5498,7 +5495,7 @@
         <v>54000</v>
       </c>
       <c r="L7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5512,7 +5509,7 @@
         <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J8">
         <v>-1</v>
@@ -5521,7 +5518,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
         <v>106</v>
@@ -5546,7 +5543,7 @@
         <v>37000</v>
       </c>
       <c r="L9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -5569,16 +5566,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
         <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
         <v>76</v>
@@ -5594,15 +5591,15 @@
         <v>29000</v>
       </c>
       <c r="L11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
         <v>77</v>
@@ -5624,21 +5621,21 @@
         <v>23000</v>
       </c>
       <c r="L12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
         <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
         <v>76</v>
@@ -5654,15 +5651,15 @@
         <v>7000</v>
       </c>
       <c r="L13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
         <v>77</v>
@@ -5684,12 +5681,12 @@
         <v>5000</v>
       </c>
       <c r="L14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
         <v>87</v>
@@ -5698,7 +5695,7 @@
         <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
         <v>76</v>
@@ -5714,12 +5711,12 @@
         <v>40000</v>
       </c>
       <c r="L15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
         <v>87</v>
@@ -5744,21 +5741,21 @@
         <v>20000</v>
       </c>
       <c r="L16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
         <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
         <v>76</v>
@@ -5774,15 +5771,15 @@
         <v>30000</v>
       </c>
       <c r="L17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
         <v>77</v>
@@ -5804,7 +5801,7 @@
         <v>24000</v>
       </c>
       <c r="L18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5818,8 +5815,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5937,7 +5934,7 @@
         <v>54000</v>
       </c>
       <c r="L7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5951,7 +5948,7 @@
         <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J8">
         <v>-1</v>
@@ -5985,7 +5982,7 @@
         <v>37000</v>
       </c>
       <c r="L9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6008,16 +6005,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="s">
         <v>114</v>
-      </c>
-      <c r="C11" t="s">
-        <v>115</v>
       </c>
       <c r="D11" t="s">
         <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G11" t="s">
         <v>76</v>
@@ -6033,15 +6030,15 @@
         <v>29000</v>
       </c>
       <c r="L11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
         <v>77</v>
@@ -6063,21 +6060,21 @@
         <v>23000</v>
       </c>
       <c r="L12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
         <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
         <v>76</v>
@@ -6093,15 +6090,15 @@
         <v>7000</v>
       </c>
       <c r="L13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
         <v>77</v>
@@ -6123,12 +6120,12 @@
         <v>5000</v>
       </c>
       <c r="L14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
         <v>87</v>
@@ -6137,7 +6134,7 @@
         <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
         <v>76</v>
@@ -6153,12 +6150,12 @@
         <v>40000</v>
       </c>
       <c r="L15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
         <v>87</v>
@@ -6183,21 +6180,21 @@
         <v>20000</v>
       </c>
       <c r="L16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
         <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
         <v>76</v>
@@ -6213,15 +6210,15 @@
         <v>30000</v>
       </c>
       <c r="L17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
         <v>77</v>
@@ -6243,7 +6240,7 @@
         <v>24000</v>
       </c>
       <c r="L18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add DH Storage and tidy some files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF18B8F9-36B2-4868-B09F-38EEA1339FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E4907-7F3E-47D2-807A-B6E4A5DAB150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -110,7 +110,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -5263,7 +5262,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -5816,10 +5815,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6037,212 +6036,224 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="J12">
+        <v>-1</v>
+      </c>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>121</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>115</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>77</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>104</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>76</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>68</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>1</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K13" s="17">
         <f>config!D8*1000</f>
         <v>23000</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>118</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>116</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>77</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>108</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G15" t="s">
         <v>76</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H15" t="s">
         <v>68</v>
       </c>
-      <c r="I13">
+      <c r="I15">
         <v>1</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K15" s="17">
         <f>config!C9*1000</f>
         <v>7000</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>122</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>116</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>77</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>104</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G16" t="s">
         <v>76</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H16" t="s">
         <v>68</v>
       </c>
-      <c r="I14">
+      <c r="I16">
         <v>1</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K16" s="17">
         <f>config!D9*1000</f>
         <v>5000</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>119</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>87</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>77</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" t="s">
         <v>108</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>76</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>68</v>
       </c>
-      <c r="I15">
+      <c r="I17">
         <v>1</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K17" s="17">
         <f>config!C6*1000</f>
         <v>40000</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>123</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>87</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>77</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>104</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>76</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H18" t="s">
         <v>68</v>
       </c>
-      <c r="I16">
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K18" s="17">
         <f>config!D6*1000</f>
         <v>20000</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L18" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>120</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>117</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
         <v>108</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G19" t="s">
         <v>76</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>68</v>
       </c>
-      <c r="I17">
+      <c r="I19">
         <v>1</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K19" s="17">
         <f>config!C10*1000</f>
         <v>30000</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>124</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>117</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>77</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>104</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G20" t="s">
         <v>76</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>68</v>
       </c>
-      <c r="I18">
+      <c r="I20">
         <v>1</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K20" s="17">
         <f>config!D10*1000</f>
         <v>24000</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L20" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DH cost update and RSD CBs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BAAD37-9F1E-49B1-98FD-B7426EEEB49A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C4D157-2CBB-4B35-8621-FB1A434CAF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="172">
   <si>
     <t>LimType</t>
   </si>
@@ -634,6 +634,48 @@
   <si>
     <t>Services</t>
   </si>
+  <si>
+    <t>2031-2035</t>
+  </si>
+  <si>
+    <t>2036-2040</t>
+  </si>
+  <si>
+    <t>2041-2046</t>
+  </si>
+  <si>
+    <t>2046-2050</t>
+  </si>
+  <si>
+    <t>initial sectoral Forecast Total</t>
+  </si>
+  <si>
+    <t>2041-2045</t>
+  </si>
+  <si>
+    <t>UC_SCB_RSD_2031-2035_Single</t>
+  </si>
+  <si>
+    <t>UC_SCB_RSD_2036-2040_Single</t>
+  </si>
+  <si>
+    <t>UC_SCB_RSD_2041-2045_Single</t>
+  </si>
+  <si>
+    <t>UC_SCB_RSD_2046-2050_Single</t>
+  </si>
+  <si>
+    <t>RSD Carbon Budget-2031-2035- Single</t>
+  </si>
+  <si>
+    <t>RSD Carbon Budget-2036-2040- Single</t>
+  </si>
+  <si>
+    <t>RSD Carbon Budget-2041-2045- Single</t>
+  </si>
+  <si>
+    <t>RSD Carbon Budget-2046-2050- Single</t>
+  </si>
 </sst>
 </file>
 
@@ -642,7 +684,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,8 +802,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +862,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,7 +945,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -968,6 +1023,10 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4493,7 +4552,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5257,10 +5316,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B3:D13"/>
+  <dimension ref="B3:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5268,24 +5327,37 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>108</v>
       </c>
@@ -5295,8 +5367,24 @@
       <c r="D6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="37">
+        <f>FORECAST($E$13,C6:D6,$C$13:$D$13)*($E$13/$E$17)</f>
+        <v>8.4265437340774003</v>
+      </c>
+      <c r="F6" s="36">
+        <f>FORECAST($F$13,C6:E6,$C$13:$E$13)*($F$13/$F$17)</f>
+        <v>0.48421081131070487</v>
+      </c>
+      <c r="G6" s="36">
+        <f>FORECAST($G$13,C6:F6,$C$13:$F$13)*($G$13/$G$17)</f>
+        <v>-6.6326481774698269</v>
+      </c>
+      <c r="H6" s="36">
+        <f>FORECAST($H$13,C6:G6,$C$13:$G$13)*($H$13/$H$17)</f>
+        <v>-11.848838833375311</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>109</v>
       </c>
@@ -5306,8 +5394,24 @@
       <c r="D7">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="37">
+        <f t="shared" ref="E7:E11" si="0">FORECAST($E$13,C7:D7,$C$13:$D$13)*($E$13/$E$17)</f>
+        <v>24.565206842169111</v>
+      </c>
+      <c r="F7" s="36">
+        <f t="shared" ref="F7:F11" si="1">FORECAST($F$13,C7:E7,$C$13:$E$13)*($F$13/$F$17)</f>
+        <v>15.93562877648943</v>
+      </c>
+      <c r="G7" s="36">
+        <f t="shared" ref="G7:G11" si="2">FORECAST($G$13,C7:F7,$C$13:$F$13)*($G$13/$G$17)</f>
+        <v>7.6580236243288446</v>
+      </c>
+      <c r="H7" s="36">
+        <f t="shared" ref="H7:H11" si="3">FORECAST($H$13,C7:G7,$C$13:$G$13)*($H$13/$H$17)</f>
+        <v>0.19084233076914464</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>156</v>
       </c>
@@ -5317,8 +5421,24 @@
       <c r="D8">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="37">
+        <f t="shared" si="0"/>
+        <v>17.320211088196046</v>
+      </c>
+      <c r="F8" s="36">
+        <f t="shared" si="1"/>
+        <v>13.340705392237242</v>
+      </c>
+      <c r="G8" s="36">
+        <f t="shared" si="2"/>
+        <v>9.3116139356605139</v>
+      </c>
+      <c r="H8" s="36">
+        <f t="shared" si="3"/>
+        <v>5.1683503882548392</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>157</v>
       </c>
@@ -5328,8 +5448,24 @@
       <c r="D9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="37">
+        <f t="shared" si="0"/>
+        <v>3.4530510736382389</v>
+      </c>
+      <c r="F9" s="36">
+        <f t="shared" si="1"/>
+        <v>2.3770285191623697</v>
+      </c>
+      <c r="G9" s="36">
+        <f t="shared" si="2"/>
+        <v>1.3311013685297457</v>
+      </c>
+      <c r="H9" s="36">
+        <f t="shared" si="3"/>
+        <v>0.35446941753319205</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>110</v>
       </c>
@@ -5339,8 +5475,24 @@
       <c r="D10">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="37">
+        <f t="shared" si="0"/>
+        <v>18.19034332160621</v>
+      </c>
+      <c r="F10" s="36">
+        <f t="shared" si="1"/>
+        <v>14.116907871581002</v>
+      </c>
+      <c r="G10" s="36">
+        <f t="shared" si="2"/>
+        <v>9.9764026644194228</v>
+      </c>
+      <c r="H10" s="36">
+        <f t="shared" si="3"/>
+        <v>5.6814681552117428</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>111</v>
       </c>
@@ -5350,32 +5502,82 @@
       <c r="D11">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="37">
+        <f t="shared" si="0"/>
+        <v>79.044643940312994</v>
+      </c>
+      <c r="F11" s="36">
+        <f t="shared" si="1"/>
+        <v>66.995518629219248</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="2"/>
+        <v>53.855506584531291</v>
+      </c>
+      <c r="H11" s="36">
+        <f t="shared" si="3"/>
+        <v>38.203708541606396</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>295</v>
       </c>
       <c r="D13">
         <v>200</v>
       </c>
+      <c r="E13">
+        <v>151</v>
+      </c>
+      <c r="F13" s="37">
+        <f>E13*0.75</f>
+        <v>113.25</v>
+      </c>
+      <c r="G13" s="37">
+        <f>E13*0.5</f>
+        <v>75.5</v>
+      </c>
+      <c r="H13" s="37">
+        <f>E13*0.25</f>
+        <v>37.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>173.53684210526316</v>
+      </c>
+      <c r="F17">
+        <v>127.97926901312107</v>
+      </c>
+      <c r="G17">
+        <v>87.997655376113414</v>
+      </c>
+      <c r="H17">
+        <v>48.763131978627342</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -5624,186 +5826,315 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="38">
+        <v>1</v>
+      </c>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39">
+        <f>config!E8*1000</f>
+        <v>17320.211088196047</v>
+      </c>
+      <c r="L13" s="38" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="38">
+        <v>1</v>
+      </c>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39">
+        <f>config!F8*1000</f>
+        <v>13340.705392237242</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="38">
+        <v>1</v>
+      </c>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39">
+        <f>config!G8*1000</f>
+        <v>9311.6139356605145</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="38">
+        <v>1</v>
+      </c>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39">
+        <f>config!H8*1000</f>
+        <v>5168.3503882548393</v>
+      </c>
+      <c r="L16" s="38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>138</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C17" t="s">
         <v>115</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D17" t="s">
         <v>77</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F17" t="s">
         <v>103</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G17" t="s">
         <v>76</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H17" t="s">
         <v>68</v>
       </c>
-      <c r="I13">
+      <c r="I17">
         <v>1</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K17" s="17">
         <f>config!C9*1000</f>
         <v>7000</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L17" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>139</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C18" t="s">
         <v>115</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D18" t="s">
         <v>77</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F18" t="s">
         <v>104</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G18" t="s">
         <v>76</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H18" t="s">
         <v>68</v>
       </c>
-      <c r="I14">
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K18" s="17">
         <f>config!D9*1000</f>
         <v>5000</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L18" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>140</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C19" t="s">
         <v>87</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D19" t="s">
         <v>77</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F19" t="s">
         <v>103</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G19" t="s">
         <v>76</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H19" t="s">
         <v>68</v>
       </c>
-      <c r="I15">
+      <c r="I19">
         <v>1</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K19" s="17">
         <f>config!C6*1000</f>
         <v>40000</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L19" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>141</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D20" t="s">
         <v>77</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F20" t="s">
         <v>104</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G20" t="s">
         <v>76</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H20" t="s">
         <v>68</v>
       </c>
-      <c r="I16">
+      <c r="I20">
         <v>1</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K20" s="17">
         <f>config!D6*1000</f>
         <v>20000</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L20" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>142</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>116</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D21" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F21" t="s">
         <v>103</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G21" t="s">
         <v>76</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H21" t="s">
         <v>68</v>
       </c>
-      <c r="I17">
+      <c r="I21">
         <v>1</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K21" s="17">
         <f>config!C10*1000</f>
         <v>30000</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L21" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>143</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C22" t="s">
         <v>116</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D22" t="s">
         <v>77</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F22" t="s">
         <v>104</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G22" t="s">
         <v>76</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H22" t="s">
         <v>68</v>
       </c>
-      <c r="I18">
+      <c r="I22">
         <v>1</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K22" s="17">
         <f>config!D10*1000</f>
         <v>24000</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L22" t="s">
         <v>153</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
model not running - increase RSD CBS by 20%
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_Sector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E4DDE6-6B8E-433A-A8B0-D7BC6849AD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3512A3B-50E8-42F1-95C9-9A415F86657B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5578,7 +5578,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5850,8 +5850,8 @@
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="36">
-        <f>config!E8*1000</f>
-        <v>17320.211088196047</v>
+        <f>config!E8*1000*1.2</f>
+        <v>20784.253305835256</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>164</v>
@@ -5882,8 +5882,8 @@
       </c>
       <c r="J14" s="35"/>
       <c r="K14" s="36">
-        <f>config!F8*1000</f>
-        <v>13340.705392237242</v>
+        <f>config!F8*1000*1.2</f>
+        <v>16008.84647068469</v>
       </c>
       <c r="L14" s="35" t="s">
         <v>165</v>
@@ -5914,8 +5914,8 @@
       </c>
       <c r="J15" s="35"/>
       <c r="K15" s="36">
-        <f>config!G8*1000</f>
-        <v>9311.6139356605145</v>
+        <f>config!G8*1000*1.2</f>
+        <v>11173.936722792618</v>
       </c>
       <c r="L15" s="35" t="s">
         <v>166</v>
@@ -5946,8 +5946,8 @@
       </c>
       <c r="J16" s="35"/>
       <c r="K16" s="36">
-        <f>config!H8*1000</f>
-        <v>5168.3503882548393</v>
+        <f>config!H8*1000*1.2</f>
+        <v>6202.0204659058072</v>
       </c>
       <c r="L16" s="35" t="s">
         <v>167</v>

</xml_diff>